<commit_message>
Fix issue if excel ID list is empty
</commit_message>
<xml_diff>
--- a/example_td.xlsx
+++ b/example_td.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\automation-boilerplate-main\automation-boilerplate-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieKarlsson\Project\github\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA14A0CE-DD84-4EED-9323-64814B1CBD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FE5945-FC37-4676-AF08-260A8BC47FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -42,8 +42,6 @@
     <definedName name="_Toc519497422" localSheetId="0">Overview!$E$4</definedName>
     <definedName name="Activity">[1]Data!$G$2:$G$23</definedName>
     <definedName name="Akt">[1]Data!$B$2:$B$17</definedName>
-    <definedName name="projno17">[2]Data!$A$2:$A$188</definedName>
-    <definedName name="projnr">[1]Data!$A$2:$A$140</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$3:$D$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">AI!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="9">Alarm!$3:$3</definedName>
@@ -54,6 +52,8 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="7">PID!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">Sum!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Valve!$3:$3</definedName>
+    <definedName name="projno17">[2]Data!$A$2:$A$188</definedName>
+    <definedName name="projnr">[1]Data!$A$2:$A$140</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4494,7 +4494,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4797,15 +4797,15 @@
       <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="2" customWidth="1"/>
-    <col min="5" max="6" width="15.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="15.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="3" customWidth="1"/>
-    <col min="11" max="1024" width="9.140625" style="3"/>
+    <col min="1" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="15.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="15.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" style="3" customWidth="1"/>
+    <col min="11" max="1024" width="9.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" ht="32.25" customHeight="1">
@@ -4868,7 +4868,7 @@
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="4" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
@@ -4903,7 +4903,7 @@
       <c r="I4" s="20"/>
       <c r="J4" s="21"/>
     </row>
-    <row r="5" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="5" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>13</v>
       </c>
@@ -4938,7 +4938,7 @@
       <c r="I5" s="23"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="6" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A6" s="22" t="s">
         <v>14</v>
       </c>
@@ -4964,7 +4964,7 @@
       <c r="I6" s="23"/>
       <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="7" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A7" s="22" t="s">
         <v>15</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="I7" s="23"/>
       <c r="J7" s="21"/>
     </row>
-    <row r="8" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="8" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A8" s="22" t="s">
         <v>16</v>
       </c>
@@ -5019,7 +5019,7 @@
       <c r="I8" s="23"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="9" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A9" s="22" t="s">
         <v>17</v>
       </c>
@@ -5048,7 +5048,7 @@
       <c r="I9" s="23"/>
       <c r="J9" s="21"/>
     </row>
-    <row r="10" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="10" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A10" s="22" t="s">
         <v>18</v>
       </c>
@@ -5074,7 +5074,7 @@
       <c r="I10" s="23"/>
       <c r="J10" s="21"/>
     </row>
-    <row r="11" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="11" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A11" s="22" t="s">
         <v>9</v>
       </c>
@@ -5094,28 +5094,28 @@
       <c r="I11" s="23"/>
       <c r="J11" s="21"/>
     </row>
-    <row r="12" spans="1:10" ht="25.15" customHeight="1">
+    <row r="12" spans="1:10" ht="25.2" customHeight="1">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="25.15" customHeight="1">
+    <row r="13" spans="1:10" ht="25.2" customHeight="1">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="25.15" customHeight="1">
+    <row r="14" spans="1:10" ht="25.2" customHeight="1">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="25.15" customHeight="1">
+    <row r="15" spans="1:10" ht="25.2" customHeight="1">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="25.15" customHeight="1">
+    <row r="16" spans="1:10" ht="25.2" customHeight="1">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="25.15" customHeight="1">
+    <row r="17" spans="1:10" ht="25.2" customHeight="1">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="25.15" customHeight="1">
+    <row r="18" spans="1:10" ht="25.2" customHeight="1">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="25.15" customHeight="1">
+    <row r="19" spans="1:10" ht="25.2" customHeight="1">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -5146,7 +5146,7 @@
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
     </row>
-    <row r="22" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="22" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>20</v>
       </c>
@@ -5162,7 +5162,7 @@
       <c r="I22" s="56"/>
       <c r="J22" s="56"/>
     </row>
-    <row r="23" spans="1:10" s="18" customFormat="1" ht="25.15" customHeight="1">
+    <row r="23" spans="1:10" s="18" customFormat="1" ht="25.2" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>22</v>
       </c>
@@ -5313,26 +5313,26 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="26"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="17" width="9.109375" style="26"/>
     <col min="18" max="18" width="12" style="26" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="26"/>
-    <col min="20" max="20" width="21.7109375" style="26" customWidth="1"/>
-    <col min="21" max="1024" width="9.140625" style="26"/>
+    <col min="19" max="19" width="9.109375" style="26"/>
+    <col min="20" max="20" width="21.6640625" style="26" customWidth="1"/>
+    <col min="21" max="1024" width="9.109375" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.899999999999999" customHeight="1">
+    <row r="1" spans="1:15" ht="19.95" customHeight="1">
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -5349,7 +5349,7 @@
       <c r="N1" s="28"/>
       <c r="O1" s="29"/>
     </row>
-    <row r="2" spans="1:15" ht="19.899999999999999" customHeight="1">
+    <row r="2" spans="1:15" ht="19.95" customHeight="1">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
@@ -10624,33 +10624,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AME299"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="26"/>
-    <col min="19" max="19" width="11.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="20" max="1016" width="9.140625" style="26"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" style="26"/>
+    <col min="19" max="19" width="11.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="1016" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1019">
@@ -10729,7 +10729,7 @@
       <c r="P2" s="51"/>
       <c r="Q2" s="51"/>
     </row>
-    <row r="3" spans="1:1019" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="3" spans="1:1019" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A3" s="30" t="s">
         <v>24</v>
       </c>
@@ -10786,7 +10786,7 @@
       <c r="AMD3"/>
       <c r="AME3"/>
     </row>
-    <row r="4" spans="1:1019" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="4" spans="1:1019" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A4" s="32"/>
       <c r="B4" s="58">
         <f>COUNTA(B6:B299)</f>
@@ -10835,7 +10835,7 @@
       <c r="AMD4"/>
       <c r="AME4"/>
     </row>
-    <row r="5" spans="1:1019" ht="15.75" thickBot="1">
+    <row r="5" spans="1:1019" ht="15" thickBot="1">
       <c r="A5" s="36"/>
       <c r="B5" s="58"/>
       <c r="C5" s="36"/>
@@ -16977,26 +16977,26 @@
       <selection pane="bottomLeft" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.28515625" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="26"/>
-    <col min="18" max="18" width="11.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="19" max="1017" width="9.140625" style="26"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.33203125" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="26"/>
+    <col min="18" max="18" width="11.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="1017" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018">
@@ -22749,23 +22749,23 @@
       <selection pane="bottomLeft" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" customWidth="1"/>
     <col min="15" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="26"/>
-    <col min="18" max="18" width="11.85546875" style="26" customWidth="1"/>
-    <col min="19" max="1017" width="9.140625" style="26"/>
+    <col min="17" max="17" width="9.109375" style="26"/>
+    <col min="18" max="18" width="11.88671875" style="26" customWidth="1"/>
+    <col min="19" max="1017" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -28633,25 +28633,25 @@
       <selection pane="bottomLeft" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.28515625" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="26"/>
-    <col min="18" max="18" width="13.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="19" max="1020" width="9.140625" style="26"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.33203125" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="26"/>
+    <col min="18" max="18" width="13.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="1020" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -28726,7 +28726,7 @@
       <c r="O2" s="52"/>
       <c r="P2" s="52"/>
     </row>
-    <row r="3" spans="1:18" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="3" spans="1:18" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A3" s="30" t="s">
         <v>24</v>
       </c>
@@ -28777,7 +28777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="4" spans="1:18" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A4" s="32"/>
       <c r="B4" s="58">
         <f>COUNTA(B6:B300)</f>
@@ -28819,7 +28819,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1">
+    <row r="5" spans="1:18" ht="15" thickBot="1">
       <c r="A5" s="36"/>
       <c r="B5" s="58"/>
       <c r="C5" s="36"/>
@@ -34305,29 +34305,29 @@
       <selection pane="bottomLeft" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="26"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="26"/>
     <col min="18" max="18" width="12" style="26" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="26"/>
-    <col min="20" max="20" width="21.7109375" style="26" customWidth="1"/>
-    <col min="21" max="1022" width="9.140625" style="26"/>
+    <col min="19" max="19" width="9.109375" style="26"/>
+    <col min="20" max="20" width="21.6640625" style="26" customWidth="1"/>
+    <col min="21" max="1022" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1023">
@@ -34408,7 +34408,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="3" spans="1:1023" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A3" s="30" t="s">
         <v>24</v>
       </c>
@@ -34459,7 +34459,7 @@
       </c>
       <c r="AMI3"/>
     </row>
-    <row r="4" spans="1:1023" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="4" spans="1:1023" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A4" s="32"/>
       <c r="B4" s="58">
         <f>COUNTA(B6:B300)</f>
@@ -34499,7 +34499,7 @@
       <c r="P4" s="34"/>
       <c r="AMI4"/>
     </row>
-    <row r="5" spans="1:1023" ht="15.75" thickBot="1">
+    <row r="5" spans="1:1023" ht="15" thickBot="1">
       <c r="A5" s="36"/>
       <c r="B5" s="58"/>
       <c r="C5" s="36"/>
@@ -40424,29 +40424,29 @@
       <selection pane="bottomLeft" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" style="26"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.109375" style="26"/>
     <col min="19" max="19" width="12" style="26" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="26"/>
-    <col min="21" max="21" width="21.7109375" style="26" customWidth="1"/>
-    <col min="22" max="1025" width="9.140625" style="26"/>
+    <col min="20" max="20" width="9.109375" style="26"/>
+    <col min="21" max="21" width="21.6640625" style="26" customWidth="1"/>
+    <col min="22" max="1025" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -46271,30 +46271,30 @@
       <selection pane="bottomLeft" sqref="A1:T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="6.44140625" customWidth="1"/>
     <col min="21" max="21" width="12" style="26" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="26"/>
-    <col min="23" max="23" width="21.7109375" style="26" customWidth="1"/>
-    <col min="24" max="1026" width="9.140625" style="26"/>
+    <col min="22" max="22" width="9.109375" style="26"/>
+    <col min="23" max="23" width="21.6640625" style="26" customWidth="1"/>
+    <col min="24" max="1026" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -46391,7 +46391,7 @@
       <c r="S2" s="52"/>
       <c r="T2" s="52"/>
     </row>
-    <row r="3" spans="1:20" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="3" spans="1:20" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A3" s="30" t="s">
         <v>24</v>
       </c>
@@ -46449,7 +46449,7 @@
       <c r="S3" s="57"/>
       <c r="T3" s="57"/>
     </row>
-    <row r="4" spans="1:20" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="4" spans="1:20" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A4" s="32"/>
       <c r="B4" s="58">
         <f>COUNTA(B6:B300)</f>
@@ -46495,7 +46495,7 @@
       <c r="S4" s="33"/>
       <c r="T4" s="34"/>
     </row>
-    <row r="5" spans="1:20" ht="15.75" thickBot="1">
+    <row r="5" spans="1:20" ht="15" thickBot="1">
       <c r="A5" s="36"/>
       <c r="B5" s="58"/>
       <c r="C5" s="36"/>
@@ -53234,29 +53234,29 @@
       <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" style="26"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.109375" style="26"/>
     <col min="19" max="19" width="12" style="26" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="26"/>
-    <col min="21" max="21" width="21.7109375" style="26" customWidth="1"/>
-    <col min="22" max="1025" width="9.140625" style="26"/>
+    <col min="20" max="20" width="9.109375" style="26"/>
+    <col min="21" max="21" width="21.6640625" style="26" customWidth="1"/>
+    <col min="22" max="1025" width="9.109375" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -53337,7 +53337,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="3" spans="1:16" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A3" s="49" t="s">
         <v>24</v>
       </c>
@@ -53387,7 +53387,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="4" spans="1:16" s="31" customFormat="1" ht="15" thickBot="1">
       <c r="A4" s="32"/>
       <c r="B4" s="58">
         <f>COUNTA(B6:B300)</f>
@@ -53426,7 +53426,7 @@
       <c r="O4" s="33"/>
       <c r="P4" s="34"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" thickBot="1">
+    <row r="5" spans="1:16" ht="15" thickBot="1">
       <c r="A5" s="36"/>
       <c r="B5" s="58"/>
       <c r="C5" s="36"/>

</xml_diff>

<commit_message>
Delat upp DB generering i PLC mappar, lagt till ASI Block generering ej testat, alarm comment plc fixad
Delat upp DB generering i PLC mappar, lagt till ASI Block generering ej testat, alarm comment plc fixad
</commit_message>
<xml_diff>
--- a/example_td.xlsx
+++ b/example_td.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieKarlsson\Documents\MC Doc\TD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Generator\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB46E5B1-D031-44AD-B452-2974FB1A0026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994B1306-1A64-4C1F-A790-7EAAA2F83488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{B894503C-AA65-4B2C-BD25-60E31CA889FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B894503C-AA65-4B2C-BD25-60E31CA889FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="395">
   <si>
     <t>Sheet</t>
   </si>
@@ -1420,6 +1420,99 @@
 • Cleanup, remove unneccessary data, improve look &amp; feel
 • Utilize name manager in excel to decrease coupling between sheets
 • Update Configurations sheet, use named tables instead of hardcoded reference</t>
+  </si>
+  <si>
+    <t>ASI Master</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>11A</t>
+  </si>
+  <si>
+    <t>12A</t>
+  </si>
+  <si>
+    <t>13A</t>
+  </si>
+  <si>
+    <t>14A</t>
+  </si>
+  <si>
+    <t>15A</t>
+  </si>
+  <si>
+    <t>16A</t>
+  </si>
+  <si>
+    <t>17A</t>
+  </si>
+  <si>
+    <t>18A</t>
+  </si>
+  <si>
+    <t>19A</t>
+  </si>
+  <si>
+    <t>20A</t>
+  </si>
+  <si>
+    <t>21A</t>
+  </si>
+  <si>
+    <t>22A</t>
+  </si>
+  <si>
+    <t>23A</t>
+  </si>
+  <si>
+    <t>24A</t>
+  </si>
+  <si>
+    <t>ASI Addr</t>
+  </si>
+  <si>
+    <t>AS100</t>
+  </si>
+  <si>
+    <t>AS200</t>
+  </si>
+  <si>
+    <t>AS300</t>
+  </si>
+  <si>
+    <t>AS400</t>
+  </si>
+  <si>
+    <t>AS500</t>
   </si>
 </sst>
 </file>
@@ -5779,7 +5872,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6078,7 +6171,7 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:AMC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -11925,9 +12018,9 @@
   <sheetPr codeName="Blad3"/>
   <dimension ref="A1:ALI293"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6:C26"/>
+      <selection pane="bottomLeft" activeCell="N6" sqref="N6:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -12020,6 +12113,12 @@
       <c r="L3" s="45" t="s">
         <v>212</v>
       </c>
+      <c r="M3" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>364</v>
+      </c>
       <c r="ALG3"/>
       <c r="ALH3"/>
       <c r="ALI3"/>
@@ -12114,6 +12213,12 @@
         <f>IF(ISBLANK(F6),"",VLOOKUP(F6,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
+      <c r="M6" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="7" spans="1:997">
       <c r="A7" s="35"/>
@@ -12141,6 +12246,12 @@
         <f>IF(ISBLANK(F7),"",VLOOKUP(F7,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
+      <c r="M7" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="8" spans="1:997">
       <c r="A8" s="35"/>
@@ -12168,6 +12279,12 @@
         <f>IF(ISBLANK(F8),"",VLOOKUP(F8,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
+      <c r="M8" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="9" spans="1:997">
       <c r="A9" s="35"/>
@@ -12195,6 +12312,12 @@
         <f>IF(ISBLANK(F9),"",VLOOKUP(F9,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
+      <c r="M9" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="10" spans="1:997">
       <c r="A10" s="35"/>
@@ -12222,6 +12345,12 @@
         <f>IF(ISBLANK(F10),"",VLOOKUP(F10,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
+      <c r="M10" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="11" spans="1:997">
       <c r="A11" s="35"/>
@@ -12249,6 +12378,12 @@
         <f>IF(ISBLANK(F11),"",VLOOKUP(F11,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
+      <c r="M11" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="12" spans="1:997">
       <c r="A12" s="35"/>
@@ -12276,6 +12411,12 @@
         <f>IF(ISBLANK(F12),"",VLOOKUP(F12,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
+      <c r="M12" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="13" spans="1:997">
       <c r="A13" s="35"/>
@@ -12303,6 +12444,12 @@
         <f>IF(ISBLANK(F13),"",VLOOKUP(F13,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
+      <c r="M13" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="14" spans="1:997">
       <c r="A14" s="35"/>
@@ -12330,6 +12477,12 @@
         <f>IF(ISBLANK(F14),"",VLOOKUP(F14,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
+      <c r="M14" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="15" spans="1:997">
       <c r="A15" s="35"/>
@@ -12357,6 +12510,12 @@
         <f>IF(ISBLANK(F15),"",VLOOKUP(F15,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
+      <c r="M15" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="16" spans="1:997">
       <c r="A16" s="35"/>
@@ -12384,8 +12543,14 @@
         <f>IF(ISBLANK(F16),"",VLOOKUP(F16,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="35"/>
       <c r="B17" s="37" t="s">
         <v>31</v>
@@ -12411,8 +12576,14 @@
         <f>IF(ISBLANK(F17),"",VLOOKUP(F17,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="35"/>
       <c r="B18" s="37" t="s">
         <v>32</v>
@@ -12438,8 +12609,14 @@
         <f>IF(ISBLANK(F18),"",VLOOKUP(F18,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="N18" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="35"/>
       <c r="B19" s="37" t="s">
         <v>33</v>
@@ -12465,8 +12642,14 @@
         <f>IF(ISBLANK(F19),"",VLOOKUP(F19,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="35"/>
       <c r="B20" s="37" t="s">
         <v>87</v>
@@ -12492,8 +12675,14 @@
         <f>IF(ISBLANK(F20),"",VLOOKUP(F20,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="35"/>
       <c r="B21" s="37" t="s">
         <v>88</v>
@@ -12519,8 +12708,14 @@
         <f>IF(ISBLANK(F21),"",VLOOKUP(F21,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="N21" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="35"/>
       <c r="B22" s="37" t="s">
         <v>89</v>
@@ -12546,8 +12741,14 @@
         <f>IF(ISBLANK(F22),"",VLOOKUP(F22,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="N22" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="35"/>
       <c r="B23" s="37" t="s">
         <v>90</v>
@@ -12573,8 +12774,14 @@
         <f>IF(ISBLANK(F23),"",VLOOKUP(F23,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="N23" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="35"/>
       <c r="B24" s="37" t="s">
         <v>91</v>
@@ -12600,8 +12807,14 @@
         <f>IF(ISBLANK(F24),"",VLOOKUP(F24,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="35"/>
       <c r="B25" s="37" t="s">
         <v>92</v>
@@ -12627,8 +12840,14 @@
         <f>IF(ISBLANK(F25),"",VLOOKUP(F25,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="N25" s="21" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="35"/>
       <c r="B26" s="37" t="s">
         <v>93</v>
@@ -12654,8 +12873,14 @@
         <f>IF(ISBLANK(F26),"",VLOOKUP(F26,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="35"/>
       <c r="B27" s="37" t="s">
         <v>160</v>
@@ -12681,8 +12906,14 @@
         <f>IF(ISBLANK(F27),"",VLOOKUP(F27,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="35"/>
       <c r="B28" s="37" t="s">
         <v>161</v>
@@ -12708,8 +12939,14 @@
         <f>IF(ISBLANK(F28),"",VLOOKUP(F28,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="N28" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="35"/>
       <c r="B29" s="37" t="s">
         <v>162</v>
@@ -12735,8 +12972,14 @@
         <f>IF(ISBLANK(F29),"",VLOOKUP(F29,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="N29" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="35"/>
       <c r="B30" s="37" t="s">
         <v>163</v>
@@ -12762,8 +13005,14 @@
         <f>IF(ISBLANK(F30),"",VLOOKUP(F30,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="N30" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="35"/>
       <c r="B31" s="37" t="s">
         <v>164</v>
@@ -12789,8 +13038,14 @@
         <f>IF(ISBLANK(F31),"",VLOOKUP(F31,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="N31" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="35"/>
       <c r="B32" s="37" t="s">
         <v>165</v>
@@ -12816,8 +13071,14 @@
         <f>IF(ISBLANK(F32),"",VLOOKUP(F32,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="N32" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="35"/>
       <c r="B33" s="37" t="s">
         <v>166</v>
@@ -12843,8 +13104,14 @@
         <f>IF(ISBLANK(F33),"",VLOOKUP(F33,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="N33" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="35"/>
       <c r="B34" s="37" t="s">
         <v>167</v>
@@ -12870,8 +13137,14 @@
         <f>IF(ISBLANK(F34),"",VLOOKUP(F34,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="N34" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="35"/>
       <c r="B35" s="37" t="s">
         <v>168</v>
@@ -12897,8 +13170,14 @@
         <f>IF(ISBLANK(F35),"",VLOOKUP(F35,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="N35" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="35"/>
       <c r="B36" s="37" t="s">
         <v>169</v>
@@ -12924,8 +13203,14 @@
         <f>IF(ISBLANK(F36),"",VLOOKUP(F36,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="N36" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="35"/>
       <c r="B37" s="37" t="s">
         <v>170</v>
@@ -12951,8 +13236,14 @@
         <f>IF(ISBLANK(F37),"",VLOOKUP(F37,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="N37" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="35"/>
       <c r="B38" s="37" t="s">
         <v>171</v>
@@ -12978,8 +13269,14 @@
         <f>IF(ISBLANK(F38),"",VLOOKUP(F38,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="N38" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="35"/>
       <c r="B39" s="37" t="s">
         <v>172</v>
@@ -13005,8 +13302,14 @@
         <f>IF(ISBLANK(F39),"",VLOOKUP(F39,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="N39" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="35"/>
       <c r="B40" s="37" t="s">
         <v>173</v>
@@ -13032,8 +13335,14 @@
         <f>IF(ISBLANK(F40),"",VLOOKUP(F40,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="M40" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="N40" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="35"/>
       <c r="B41" s="37" t="s">
         <v>174</v>
@@ -13059,8 +13368,14 @@
         <f>IF(ISBLANK(F41),"",VLOOKUP(F41,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="N41" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="35"/>
       <c r="B42" s="37" t="s">
         <v>175</v>
@@ -13086,8 +13401,14 @@
         <f>IF(ISBLANK(F42),"",VLOOKUP(F42,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="N42" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="35"/>
       <c r="B43" s="37" t="s">
         <v>176</v>
@@ -13113,8 +13434,14 @@
         <f>IF(ISBLANK(F43),"",VLOOKUP(F43,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="N43" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="35"/>
       <c r="B44" s="37" t="s">
         <v>177</v>
@@ -13140,8 +13467,14 @@
         <f>IF(ISBLANK(F44),"",VLOOKUP(F44,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="N44" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="35"/>
       <c r="B45" s="37" t="s">
         <v>178</v>
@@ -13167,8 +13500,14 @@
         <f>IF(ISBLANK(F45),"",VLOOKUP(F45,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45" s="21" t="s">
+        <v>383</v>
+      </c>
+      <c r="N45" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="35"/>
       <c r="B46" s="37" t="s">
         <v>179</v>
@@ -13194,8 +13533,14 @@
         <f>IF(ISBLANK(F46),"",VLOOKUP(F46,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="N46" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="35"/>
       <c r="B47" s="37" t="s">
         <v>180</v>
@@ -13221,8 +13566,14 @@
         <f>IF(ISBLANK(F47),"",VLOOKUP(F47,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="M47" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="N47" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="35"/>
       <c r="B48" s="37" t="s">
         <v>181</v>
@@ -13248,8 +13599,14 @@
         <f>IF(ISBLANK(F48),"",VLOOKUP(F48,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48" s="21" t="s">
+        <v>386</v>
+      </c>
+      <c r="N48" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="35"/>
       <c r="B49" s="37" t="s">
         <v>182</v>
@@ -13275,8 +13632,14 @@
         <f>IF(ISBLANK(F49),"",VLOOKUP(F49,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49" s="21" t="s">
+        <v>387</v>
+      </c>
+      <c r="N49" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="35"/>
       <c r="B50" s="37" t="s">
         <v>183</v>
@@ -13302,8 +13665,14 @@
         <f>IF(ISBLANK(F50),"",VLOOKUP(F50,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="N50" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" s="35"/>
       <c r="B51" s="61" t="s">
         <v>256</v>
@@ -13329,8 +13698,14 @@
         <f>IF(ISBLANK(F51),"",VLOOKUP(F51,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="N51" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" s="35"/>
       <c r="B52" s="61" t="s">
         <v>257</v>
@@ -13356,8 +13731,14 @@
         <f>IF(ISBLANK(F52),"",VLOOKUP(F52,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="M52" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="N52" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="35"/>
       <c r="B53" s="61" t="s">
         <v>258</v>
@@ -13383,8 +13764,14 @@
         <f>IF(ISBLANK(F53),"",VLOOKUP(F53,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="N53" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" s="35"/>
       <c r="B54" s="61" t="s">
         <v>259</v>
@@ -13410,8 +13797,14 @@
         <f>IF(ISBLANK(F54),"",VLOOKUP(F54,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="N54" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" s="35"/>
       <c r="B55" s="61" t="s">
         <v>260</v>
@@ -13437,8 +13830,14 @@
         <f>IF(ISBLANK(F55),"",VLOOKUP(F55,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="N55" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" s="35"/>
       <c r="B56" s="61" t="s">
         <v>261</v>
@@ -13464,8 +13863,14 @@
         <f>IF(ISBLANK(F56),"",VLOOKUP(F56,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="N56" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" s="35"/>
       <c r="B57" s="61" t="s">
         <v>262</v>
@@ -13491,8 +13896,14 @@
         <f>IF(ISBLANK(F57),"",VLOOKUP(F57,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="N57" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" s="35"/>
       <c r="B58" s="61" t="s">
         <v>263</v>
@@ -13518,8 +13929,14 @@
         <f>IF(ISBLANK(F58),"",VLOOKUP(F58,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="N58" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="35"/>
       <c r="B59" s="61" t="s">
         <v>264</v>
@@ -13545,8 +13962,14 @@
         <f>IF(ISBLANK(F59),"",VLOOKUP(F59,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="N59" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" s="35"/>
       <c r="B60" s="61" t="s">
         <v>265</v>
@@ -13572,8 +13995,14 @@
         <f>IF(ISBLANK(F60),"",VLOOKUP(F60,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="M60" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="N60" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" s="35"/>
       <c r="B61" s="61" t="s">
         <v>266</v>
@@ -13599,8 +14028,14 @@
         <f>IF(ISBLANK(F61),"",VLOOKUP(F61,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="M61" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="N61" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" s="35"/>
       <c r="B62" s="62" t="s">
         <v>267</v>
@@ -13626,8 +14061,14 @@
         <f>IF(ISBLANK(F62),"",VLOOKUP(F62,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="M62" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="N62" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" s="35"/>
       <c r="B63" s="37"/>
       <c r="C63" s="35"/>
@@ -13644,7 +14085,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:14">
       <c r="A64" s="35"/>
       <c r="B64" s="37"/>
       <c r="C64" s="35"/>

</xml_diff>

<commit_message>
ASi Code Generator fix, ASi Header replace
ASi Code was wrong structure
</commit_message>
<xml_diff>
--- a/example_td.xlsx
+++ b/example_td.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustav\Documents\GitHub\automation-boilerplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Generator\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F63FA35-4DD0-41AB-B1F1-924C8ECBBC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272A8DCC-A8C2-4E94-9E08-F3DD73D365F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{B894503C-AA65-4B2C-BD25-60E31CA889FC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B894503C-AA65-4B2C-BD25-60E31CA889FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="395">
   <si>
     <t>Sheet</t>
   </si>
@@ -1500,16 +1500,19 @@
     <t>ASI Addr</t>
   </si>
   <si>
-    <t>AS100</t>
+    <t>AS100~Master1</t>
   </si>
   <si>
-    <t>AS200</t>
+    <t>AS200~Master1</t>
   </si>
   <si>
-    <t>AS300</t>
+    <t>AS300~Master1</t>
   </si>
   <si>
-    <t>AS400</t>
+    <t>AS100_Master1_Error</t>
+  </si>
+  <si>
+    <t>AS100 ASi Master Error</t>
   </si>
 </sst>
 </file>
@@ -2687,14 +2690,14 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2745,16 +2748,383 @@
     <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Percent 2 2" xfId="9" xr:uid="{EF7A7829-79FD-4611-956F-3356E04BECF0}"/>
   </cellStyles>
-  <dxfs count="254">
+  <dxfs count="262">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Trade gothic"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F8F8"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Trade gothic"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F8F8"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4839,6 +5209,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -4923,309 +5303,6 @@
       <font>
         <color rgb="FF000000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Trade gothic"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F8F8"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Trade gothic"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F8F8"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5842,33 +5919,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}" name="valve_configs_table" displayName="valve_configs_table" ref="B3:C14" totalsRowShown="0" headerRowDxfId="253" headerRowBorderDxfId="252" tableBorderDxfId="251" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}" name="valve_configs_table" displayName="valve_configs_table" ref="B3:C14" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" headerRowCellStyle="Normal 2">
   <autoFilter ref="B3:C14" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D2B99697-6C22-4A65-9A1B-E36D1780E905}" name="Description" dataDxfId="250"/>
-    <tableColumn id="2" xr3:uid="{0C7255C4-22B6-457A-870A-411B65308579}" name="Value" dataDxfId="249"/>
+    <tableColumn id="1" xr3:uid="{D2B99697-6C22-4A65-9A1B-E36D1780E905}" name="Description" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{0C7255C4-22B6-457A-870A-411B65308579}" name="Value" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}" name="motor_configs_table" displayName="motor_configs_table" ref="E3:F7" totalsRowShown="0" headerRowDxfId="248" dataDxfId="246" headerRowBorderDxfId="247" tableBorderDxfId="245" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}" name="motor_configs_table" displayName="motor_configs_table" ref="E3:F7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" headerRowCellStyle="Normal 2">
   <autoFilter ref="E3:F7" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3566CC7F-11CE-4C21-9EB5-FA275F790C03}" name="Description" dataDxfId="244"/>
-    <tableColumn id="2" xr3:uid="{7BD42503-42BD-4F3C-A5DC-32DAB0E6CD55}" name="Value" dataDxfId="243"/>
+    <tableColumn id="1" xr3:uid="{3566CC7F-11CE-4C21-9EB5-FA275F790C03}" name="Description" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{7BD42503-42BD-4F3C-A5DC-32DAB0E6CD55}" name="Value" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}" name="alarm_configs_table" displayName="alarm_configs_table" ref="H3:I7" totalsRowShown="0" headerRowBorderDxfId="242" tableBorderDxfId="241">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}" name="alarm_configs_table" displayName="alarm_configs_table" ref="H3:I7" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="H3:I7" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{708D6350-80FE-46FF-B9B2-EC74246F1C57}" name="Description" dataDxfId="240"/>
-    <tableColumn id="2" xr3:uid="{94C6C4A0-B062-49D6-9CCC-0CD2BD3F95A4}" name="Value" dataDxfId="239"/>
+    <tableColumn id="1" xr3:uid="{708D6350-80FE-46FF-B9B2-EC74246F1C57}" name="Description" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{94C6C4A0-B062-49D6-9CCC-0CD2BD3F95A4}" name="Value" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6464,52 +6541,52 @@
     <mergeCell ref="B32:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="D6 D8:D9 F10 B4:F5 B11:F11 D12:F12">
-    <cfRule type="cellIs" dxfId="238" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="261" priority="8" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B10 B12">
-    <cfRule type="cellIs" dxfId="237" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="260" priority="14" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C10 C12">
-    <cfRule type="cellIs" dxfId="236" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="259" priority="15" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E9">
-    <cfRule type="cellIs" dxfId="235" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="258" priority="17" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F9">
-    <cfRule type="cellIs" dxfId="234" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="257" priority="18" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="233" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="256" priority="6" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="232" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="255" priority="4" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="231" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="254" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="cellIs" dxfId="230" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="253" priority="2" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="229" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="252" priority="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6558,11 +6635,11 @@
         <v>Projectnumber:</v>
       </c>
       <c r="P1" s="127"/>
-      <c r="Q1" s="124" t="str">
+      <c r="Q1" s="125" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="R1" s="125"/>
+      <c r="R1" s="126"/>
     </row>
     <row r="2" spans="1:18" ht="18" customHeight="1">
       <c r="A2" s="46"/>
@@ -6584,11 +6661,11 @@
         <v>Projectname:</v>
       </c>
       <c r="P2" s="127"/>
-      <c r="Q2" s="124" t="str">
+      <c r="Q2" s="125" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="R2" s="125"/>
+      <c r="R2" s="126"/>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="129"/>
@@ -6957,184 +7034,184 @@
     <mergeCell ref="R3:R4"/>
   </mergeCells>
   <conditionalFormatting sqref="R8:R9">
-    <cfRule type="cellIs" dxfId="62" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="201" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="202" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="203" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="204" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="58" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="213" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="214" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="215" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="216" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:F6">
-    <cfRule type="cellIs" dxfId="54" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="209" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="210" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="211" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="212" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="50" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="205" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="206" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="207" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="208" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R13:R16">
-    <cfRule type="cellIs" dxfId="46" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="189" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="190" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="191" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="192" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="42" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="197" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="198" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="199" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="200" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11:R16">
-    <cfRule type="cellIs" dxfId="38" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="193" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="194" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="195" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="196" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:F9">
-    <cfRule type="cellIs" dxfId="34" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="185" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="186" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="187" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="188" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:L9">
-    <cfRule type="cellIs" dxfId="30" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="181" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="182" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="183" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="184" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:F11">
-    <cfRule type="cellIs" dxfId="26" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="177" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="178" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="179" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="180" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:F16">
-    <cfRule type="cellIs" dxfId="22" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="173" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="174" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="175" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="176" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:L16">
-    <cfRule type="cellIs" dxfId="18" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="169" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="170" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="171" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="172" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:Q9 N11:Q16">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="7" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7153,7 +7230,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7236,9 +7313,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="24" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="A4" s="126">
+      <c r="A4" s="124">
         <f>COUNTA(A6:A296)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="107"/>
       <c r="C4" s="25"/>
@@ -7262,7 +7339,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1" thickBot="1">
-      <c r="A5" s="126"/>
+      <c r="A5" s="124"/>
       <c r="B5" s="108"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -7533,18 +7610,28 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
+      <c r="A16" s="33" t="s">
+        <v>393</v>
+      </c>
       <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="32"/>
+      <c r="C16" s="35" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>342</v>
+      </c>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
-      <c r="J16" s="74" t="str">
+      <c r="J16" s="74">
         <f>IF(ISBLANK(F16),"",VLOOKUP(F16,alarm_configs_table[],2,))</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -11753,44 +11840,44 @@
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:I296">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="14" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J296">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="between">
       <formula>750</formula>
       <formula>999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="between">
       <formula>500</formula>
       <formula>749</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="between">
       <formula>250</formula>
       <formula>499</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="between">
       <formula>1</formula>
       <formula>249</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A296">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>NOT(ISERROR(SEARCH(" ",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B296">
-    <cfRule type="duplicateValues" dxfId="1" priority="278"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="278"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F296" xr:uid="{7E766BAA-3222-4A1B-96F6-6DD936D34E56}">
@@ -12022,8 +12109,8 @@
   <dimension ref="A1:ALI282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -12037,7 +12124,7 @@
     <col min="7" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="15" style="21" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" style="21" customWidth="1"/>
     <col min="15" max="994" width="9.140625" style="21"/>
   </cols>
   <sheetData>
@@ -12057,11 +12144,11 @@
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="M1" s="124" t="str">
+      <c r="M1" s="125" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="N1" s="125"/>
+      <c r="N1" s="126"/>
     </row>
     <row r="2" spans="1:997" ht="18" customHeight="1">
       <c r="A2" s="42"/>
@@ -12079,11 +12166,11 @@
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="M2" s="124" t="str">
+      <c r="M2" s="125" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="N2" s="125"/>
+      <c r="N2" s="126"/>
     </row>
     <row r="3" spans="1:997" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -12134,7 +12221,7 @@
     </row>
     <row r="4" spans="1:997" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <f>COUNTA(B6:B282)</f>
         <v>57</v>
       </c>
@@ -12171,7 +12258,7 @@
     </row>
     <row r="5" spans="1:997" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="126"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -12524,10 +12611,10 @@
         <v>57</v>
       </c>
       <c r="M15" s="34" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:997">
@@ -12557,10 +12644,10 @@
         <v>57</v>
       </c>
       <c r="M16" s="34" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -12590,10 +12677,10 @@
         <v>57</v>
       </c>
       <c r="M17" s="34" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="N17" s="34" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -12623,10 +12710,10 @@
         <v>57</v>
       </c>
       <c r="M18" s="34" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="N18" s="34" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -12656,10 +12743,10 @@
         <v>57</v>
       </c>
       <c r="M19" s="34" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="N19" s="34" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -12688,8 +12775,12 @@
         <f>IF(ISBLANK(F20),"",VLOOKUP(F20,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
+      <c r="M20" s="34" t="s">
+        <v>379</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="35"/>
@@ -12717,8 +12808,12 @@
         <f>IF(ISBLANK(F21),"",VLOOKUP(F21,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
+      <c r="M21" s="34" t="s">
+        <v>380</v>
+      </c>
+      <c r="N21" s="34" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="35"/>
@@ -12746,8 +12841,12 @@
         <f>IF(ISBLANK(F22),"",VLOOKUP(F22,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
+      <c r="M22" s="34" t="s">
+        <v>381</v>
+      </c>
+      <c r="N22" s="34" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="35"/>
@@ -12775,8 +12874,12 @@
         <f>IF(ISBLANK(F23),"",VLOOKUP(F23,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
+      <c r="M23" s="34" t="s">
+        <v>382</v>
+      </c>
+      <c r="N23" s="34" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="35"/>
@@ -12804,8 +12907,12 @@
         <f>IF(ISBLANK(F24),"",VLOOKUP(F24,valve_configs_table[],2,))</f>
         <v>57</v>
       </c>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
+      <c r="M24" s="34" t="s">
+        <v>383</v>
+      </c>
+      <c r="N24" s="34" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="35"/>
@@ -12833,8 +12940,12 @@
         <f>IF(ISBLANK(F25),"",VLOOKUP(F25,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
+      <c r="M25" s="34" t="s">
+        <v>384</v>
+      </c>
+      <c r="N25" s="34" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="35"/>
@@ -12862,8 +12973,12 @@
         <f>IF(ISBLANK(F26),"",VLOOKUP(F26,valve_configs_table[],2,))</f>
         <v>63</v>
       </c>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
+      <c r="M26" s="34" t="s">
+        <v>385</v>
+      </c>
+      <c r="N26" s="34" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="35"/>
@@ -18238,30 +18353,30 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K282 M6:N282">
-    <cfRule type="cellIs" dxfId="228" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="224" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="247" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B13">
-    <cfRule type="duplicateValues" dxfId="223" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="246" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="222" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="245" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:B282 B7:B8 B14:B50">
-    <cfRule type="duplicateValues" dxfId="0" priority="287"/>
+    <cfRule type="duplicateValues" dxfId="244" priority="287"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F62 F282" xr:uid="{CD348D37-DD25-4857-B38F-E4611E7771B6}">
@@ -18382,7 +18497,7 @@
     </row>
     <row r="4" spans="1:1009" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <f>COUNTA(B6:B300)</f>
         <v>14</v>
       </c>
@@ -18415,7 +18530,7 @@
     </row>
     <row r="5" spans="1:1009" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="126"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -23602,86 +23717,86 @@
   </mergeCells>
   <phoneticPr fontId="36" type="noConversion"/>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="221" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="217" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="213" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J300">
-    <cfRule type="cellIs" dxfId="209" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="19" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="20" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="21" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K300">
-    <cfRule type="cellIs" dxfId="205" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8 B11:B14 B20:B300">
-    <cfRule type="duplicateValues" dxfId="201" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="223" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="200" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="222" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="199" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="221" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="198" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="220" priority="33"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F19" xr:uid="{858AD274-EE67-43BB-A3F1-3780D7923764}">
@@ -23791,7 +23906,7 @@
     </row>
     <row r="4" spans="1:9" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <f>COUNTA(B6:B303)</f>
         <v>17</v>
       </c>
@@ -23817,7 +23932,7 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="126"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -27258,75 +27373,75 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F303">
-    <cfRule type="cellIs" dxfId="197" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="195" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G303">
-    <cfRule type="cellIs" dxfId="193" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H303">
-    <cfRule type="cellIs" dxfId="189" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I303">
-    <cfRule type="cellIs" dxfId="185" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B7 B9:B10 B12:B13 B15:B16 B18:B303">
-    <cfRule type="duplicateValues" dxfId="181" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="203" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="180" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="202" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="179" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="201" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="178" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="200" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="177" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="199" priority="34"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -27424,7 +27539,7 @@
     </row>
     <row r="4" spans="1:10" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <f>COUNTA(B6:B300)</f>
         <v>1</v>
       </c>
@@ -27454,7 +27569,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="126"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -31032,77 +31147,77 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="176" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="172" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="168" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:I300">
-    <cfRule type="cellIs" dxfId="164" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J300">
-    <cfRule type="cellIs" dxfId="160" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="156" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="30"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -31147,11 +31262,11 @@
         <v>Projectnumber:</v>
       </c>
       <c r="J1" s="127"/>
-      <c r="K1" s="124" t="str">
+      <c r="K1" s="125" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="L1" s="125"/>
+      <c r="L1" s="126"/>
     </row>
     <row r="2" spans="1:1019" ht="18" customHeight="1">
       <c r="A2" s="22"/>
@@ -31167,11 +31282,11 @@
         <v>Projectname:</v>
       </c>
       <c r="J2" s="127"/>
-      <c r="K2" s="124" t="str">
+      <c r="K2" s="125" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="L2" s="125"/>
+      <c r="L2" s="126"/>
     </row>
     <row r="3" spans="1:1019" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -31214,7 +31329,7 @@
     </row>
     <row r="4" spans="1:1019" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <f>COUNTA(B6:B300)</f>
         <v>42</v>
       </c>
@@ -31244,7 +31359,7 @@
     </row>
     <row r="5" spans="1:1019" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="126"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -35965,21 +36080,21 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:I300">
-    <cfRule type="cellIs" dxfId="155" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="151" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="26"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -36025,11 +36140,11 @@
         <v>Projectnumber:</v>
       </c>
       <c r="K1" s="127"/>
-      <c r="L1" s="124" t="str">
+      <c r="L1" s="125" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="M1" s="125"/>
+      <c r="M1" s="126"/>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="43"/>
@@ -36046,11 +36161,11 @@
         <v>Projectname:</v>
       </c>
       <c r="K2" s="127"/>
-      <c r="L2" s="124" t="str">
+      <c r="L2" s="125" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="M2" s="125"/>
+      <c r="M2" s="126"/>
     </row>
     <row r="3" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -36095,7 +36210,7 @@
     </row>
     <row r="4" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <f>COUNTA(B6:B300)</f>
         <v>18</v>
       </c>
@@ -36128,7 +36243,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="126"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -40838,157 +40953,157 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="146" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="142" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="138" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6 J15:J300">
-    <cfRule type="cellIs" dxfId="134" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B300">
-    <cfRule type="duplicateValues" dxfId="130" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="129" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="128" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="127" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="126" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="125" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="121" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="117" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="113" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="47" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="48" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="49" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="50" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J14">
-    <cfRule type="cellIs" dxfId="109" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41037,11 +41152,11 @@
         <v>Projectnumber:</v>
       </c>
       <c r="L1" s="127"/>
-      <c r="M1" s="124" t="str">
+      <c r="M1" s="125" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="N1" s="125"/>
+      <c r="N1" s="126"/>
       <c r="O1" s="43"/>
       <c r="P1" s="43"/>
     </row>
@@ -41061,11 +41176,11 @@
         <v>Projectname:</v>
       </c>
       <c r="L2" s="127"/>
-      <c r="M2" s="124" t="str">
+      <c r="M2" s="125" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="N2" s="125"/>
+      <c r="N2" s="126"/>
       <c r="O2" s="43"/>
       <c r="P2" s="43"/>
     </row>
@@ -41117,7 +41232,7 @@
     </row>
     <row r="4" spans="1:16" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <f>COUNTA(B6:B299)</f>
         <v>12</v>
       </c>
@@ -41153,7 +41268,7 @@
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="126"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -46659,21 +46774,21 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:J299">
-    <cfRule type="cellIs" dxfId="105" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B299">
-    <cfRule type="duplicateValues" dxfId="101" priority="273"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="273"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -46720,11 +46835,11 @@
         <v>Projectnumber:</v>
       </c>
       <c r="K1" s="127"/>
-      <c r="L1" s="124" t="str">
+      <c r="L1" s="125" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="M1" s="125"/>
+      <c r="M1" s="126"/>
     </row>
     <row r="2" spans="1:13" s="24" customFormat="1" ht="19.5" customHeight="1">
       <c r="A2" s="43"/>
@@ -46741,11 +46856,11 @@
         <v>Projectname:</v>
       </c>
       <c r="K2" s="127"/>
-      <c r="L2" s="124" t="str">
+      <c r="L2" s="125" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="M2" s="125"/>
+      <c r="M2" s="126"/>
     </row>
     <row r="3" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="40" t="s">
@@ -46790,7 +46905,7 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <f>COUNTA(B6:B300)</f>
         <v>7</v>
       </c>
@@ -46820,7 +46935,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="126"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -51391,134 +51506,134 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="100" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="96" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="92" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="19" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="20" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="21" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6 I11:I300">
-    <cfRule type="cellIs" dxfId="88" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11 B13:B300">
-    <cfRule type="duplicateValues" dxfId="84" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="83" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="82" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="81" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="80" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="79" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="31" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="32" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="33" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="34" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="75" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="71" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="67" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>